<commit_message>
Entering table details to excel sheet has been updated
</commit_message>
<xml_diff>
--- a/Milestone Project Management.xlsx
+++ b/Milestone Project Management.xlsx
@@ -882,11 +882,29 @@
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -894,10 +912,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -921,41 +957,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -977,57 +1028,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1950,7 +1950,7 @@
                   <c:v>510.00000000000011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90.000000000000227</c:v>
+                  <c:v>810.00000000000023</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2033,11 +2033,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="-106709472"/>
-        <c:axId val="-106702944"/>
+        <c:axId val="-1308388192"/>
+        <c:axId val="-1308396896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-106709472"/>
+        <c:axId val="-1308388192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2058,7 +2058,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106702944"/>
+        <c:crossAx val="-1308396896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2066,7 +2066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-106702944"/>
+        <c:axId val="-1308396896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2087,7 +2087,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106709472"/>
+        <c:crossAx val="-1308388192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2389,7 +2389,7 @@
                   <c:v>510.00000000000011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90.000000000000227</c:v>
+                  <c:v>810.00000000000023</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2807,11 +2807,11 @@
         </c:dLbls>
         <c:gapWidth val="20"/>
         <c:overlap val="100"/>
-        <c:axId val="-106701856"/>
-        <c:axId val="-106707840"/>
+        <c:axId val="-1308383296"/>
+        <c:axId val="-1308383840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-106701856"/>
+        <c:axId val="-1308383296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2831,7 +2831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106707840"/>
+        <c:crossAx val="-1308383840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2839,7 +2839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-106707840"/>
+        <c:axId val="-1308383840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2860,7 +2860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106701856"/>
+        <c:crossAx val="-1308383296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2991,7 +2991,7 @@
                   <c:v>510.00000000000011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90.000000000000227</c:v>
+                  <c:v>810.00000000000023</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -3411,7 +3411,7 @@
                   <c:v>510.00000000000011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>90.000000000000227</c:v>
+                  <c:v>810.00000000000023</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3826,11 +3826,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-106705664"/>
-        <c:axId val="-106700768"/>
+        <c:axId val="-1308386016"/>
+        <c:axId val="-1308382752"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-106705664"/>
+        <c:axId val="-1308386016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3850,7 +3850,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106700768"/>
+        <c:crossAx val="-1308382752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3858,7 +3858,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-106700768"/>
+        <c:axId val="-1308382752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3879,7 +3879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106705664"/>
+        <c:crossAx val="-1308386016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4087,7 +4087,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1066.0000000000002</c:v>
+                  <c:v>1786.0000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>89.999999999999915</c:v>
@@ -4709,11 +4709,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-106699136"/>
-        <c:axId val="-106700224"/>
+        <c:axId val="-1308394176"/>
+        <c:axId val="-1308387104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-106699136"/>
+        <c:axId val="-1308394176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4733,7 +4733,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106700224"/>
+        <c:crossAx val="-1308387104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4741,7 +4741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-106700224"/>
+        <c:axId val="-1308387104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4761,7 +4761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106699136"/>
+        <c:crossAx val="-1308394176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4923,11 +4923,11 @@
         </c:dLbls>
         <c:gapWidth val="25"/>
         <c:overlap val="40"/>
-        <c:axId val="-106698048"/>
-        <c:axId val="-106706752"/>
+        <c:axId val="-1308386560"/>
+        <c:axId val="-1308389280"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-106698048"/>
+        <c:axId val="-1308386560"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4947,14 +4947,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106706752"/>
+        <c:crossAx val="-1308389280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-106706752"/>
+        <c:axId val="-1308389280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4975,7 +4975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-106698048"/>
+        <c:crossAx val="-1308386560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6608,8 +6608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="S49" sqref="S49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9577,23 +9577,23 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="K46" s="77">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L46" s="60">
         <f>(TaskTimings[End Time]-TaskTimings[Start Time])*1440</f>
-        <v>-570</v>
-      </c>
-      <c r="M46" s="60" t="e">
+        <v>150.00000000000003</v>
+      </c>
+      <c r="M46" s="60" t="str">
         <f>TEXT(TaskTimings[End Time]-TaskTimings[Start Time],"HH:mm")</f>
-        <v>#VALUE!</v>
+        <v>02:30</v>
       </c>
       <c r="N46" s="60">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[Date],TaskTimings[Date],TaskTimings[Employee],TaskTimings[Employee])</f>
-        <v>-570</v>
-      </c>
-      <c r="O46" s="60" t="e">
+        <v>150.00000000000003</v>
+      </c>
+      <c r="O46" s="60" t="str">
         <f>TEXT(TaskTimings[Day Total Minutes]/1440,"HH:mm")</f>
-        <v>#VALUE!</v>
+        <v>02:30</v>
       </c>
       <c r="P46" s="56" t="str">
         <f>TaskTimings[PRJ]</f>
@@ -9641,22 +9641,24 @@
       <c r="J47" s="78">
         <v>0.39583333333333331</v>
       </c>
-      <c r="K47" s="60"/>
+      <c r="K47" s="77">
+        <v>0.5</v>
+      </c>
       <c r="L47" s="60">
         <f>(TaskTimings[End Time]-TaskTimings[Start Time])*1440</f>
-        <v>-570</v>
-      </c>
-      <c r="M47" s="60" t="e">
+        <v>150.00000000000003</v>
+      </c>
+      <c r="M47" s="60" t="str">
         <f>TEXT(TaskTimings[End Time]-TaskTimings[Start Time],"HH:mm")</f>
-        <v>#VALUE!</v>
+        <v>02:30</v>
       </c>
       <c r="N47" s="60">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[Date],TaskTimings[Date],TaskTimings[Employee],TaskTimings[Employee])</f>
-        <v>-570</v>
-      </c>
-      <c r="O47" s="60" t="e">
+        <v>150.00000000000003</v>
+      </c>
+      <c r="O47" s="60" t="str">
         <f>TEXT(TaskTimings[Day Total Minutes]/1440,"HH:mm")</f>
-        <v>#VALUE!</v>
+        <v>02:30</v>
       </c>
       <c r="P47" s="56" t="str">
         <f>TaskTimings[PRJ]</f>
@@ -9698,42 +9700,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="100"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="J2" s="85" t="s">
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="J2" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="101" t="str">
+      <c r="A4" s="81" t="str">
         <f>VLOOKUP($A$1,Project[[Project]:[Project Code]],2,0)</f>
         <v>TKT</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="81"/>
       <c r="J4" s="14">
         <v>1</v>
       </c>
@@ -9757,83 +9759,83 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="81" t="s">
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="J5" s="92" t="str">
+      <c r="H5" s="91"/>
+      <c r="J5" s="84" t="str">
         <f>IFERROR(VLOOKUP(J$4,Employees[],2,0),"")</f>
         <v>Aswathy</v>
       </c>
-      <c r="K5" s="81" t="str">
+      <c r="K5" s="87" t="str">
         <f>IFERROR(VLOOKUP(K$4,Employees[],2,0),"")</f>
         <v>Vishnu</v>
       </c>
-      <c r="L5" s="81" t="str">
+      <c r="L5" s="87" t="str">
         <f>IFERROR(VLOOKUP(L$4,Employees[],2,0),"")</f>
         <v>Shareena</v>
       </c>
-      <c r="M5" s="81" t="str">
+      <c r="M5" s="87" t="str">
         <f>IFERROR(VLOOKUP(M$4,Employees[],2,0),"")</f>
         <v>Firose</v>
       </c>
-      <c r="N5" s="81" t="str">
+      <c r="N5" s="87" t="str">
         <f>IFERROR(VLOOKUP(N$4,Employees[],2,0),"")</f>
         <v/>
       </c>
-      <c r="O5" s="81" t="str">
+      <c r="O5" s="87" t="str">
         <f>IFERROR(VLOOKUP(O$4,Employees[],2,0),"")</f>
         <v/>
       </c>
-      <c r="P5" s="83" t="str">
+      <c r="P5" s="91" t="str">
         <f>IFERROR(VLOOKUP(P$4,Employees[],2,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="84"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="84"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="92"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="92"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>1</v>
       </c>
-      <c r="B7" s="96" t="str">
+      <c r="B7" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A7,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v>Database Analysis from Old Project</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="94">
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B7)</f>
         <v>375.99999999999994</v>
       </c>
-      <c r="H7" s="95"/>
+      <c r="H7" s="90"/>
       <c r="J7" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B7,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -9867,19 +9869,19 @@
       <c r="A8" s="12">
         <v>2</v>
       </c>
-      <c r="B8" s="96" t="str">
+      <c r="B8" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A8,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v>DB Designing</v>
       </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="94">
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B8)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="95"/>
+      <c r="H8" s="90"/>
       <c r="J8" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B8,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -9913,19 +9915,19 @@
       <c r="A9" s="12">
         <v>3</v>
       </c>
-      <c r="B9" s="96" t="str">
+      <c r="B9" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A9,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v>Appframe configuration</v>
       </c>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="94">
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B9)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="95"/>
+      <c r="H9" s="90"/>
       <c r="J9" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B9,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -9959,19 +9961,19 @@
       <c r="A10" s="12">
         <v>4</v>
       </c>
-      <c r="B10" s="96" t="str">
+      <c r="B10" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A10,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v>Discussion for ticketing modification</v>
       </c>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="94">
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B10)</f>
         <v>269.99999999999989</v>
       </c>
-      <c r="H10" s="95"/>
+      <c r="H10" s="90"/>
       <c r="J10" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B10,TaskTimings[Employee],J$5)</f>
         <v>90</v>
@@ -10005,19 +10007,19 @@
       <c r="A11" s="12">
         <v>5</v>
       </c>
-      <c r="B11" s="96" t="str">
+      <c r="B11" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A11,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v>Note down table relations</v>
       </c>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="94">
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B11)</f>
         <v>510.00000000000011</v>
       </c>
-      <c r="H11" s="95"/>
+      <c r="H11" s="90"/>
       <c r="J11" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B11,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10051,19 +10053,19 @@
       <c r="A12" s="12">
         <v>6</v>
       </c>
-      <c r="B12" s="96" t="str">
+      <c r="B12" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A12,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v>Entering table details into excel sheet</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="94">
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B12)</f>
-        <v>90.000000000000227</v>
-      </c>
-      <c r="H12" s="95"/>
+        <v>810.00000000000023</v>
+      </c>
+      <c r="H12" s="90"/>
       <c r="J12" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B12,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10074,7 +10076,7 @@
       </c>
       <c r="L12" s="16">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B12,TaskTimings[Employee],L$5)</f>
-        <v>90.000000000000227</v>
+        <v>810.00000000000023</v>
       </c>
       <c r="M12" s="16">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B12,TaskTimings[Employee],M$5)</f>
@@ -10097,19 +10099,19 @@
       <c r="A13" s="12">
         <v>7</v>
       </c>
-      <c r="B13" s="96" t="str">
+      <c r="B13" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A13,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="94">
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B13)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="95"/>
+      <c r="H13" s="90"/>
       <c r="J13" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B13,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10143,19 +10145,19 @@
       <c r="A14" s="12">
         <v>8</v>
       </c>
-      <c r="B14" s="96" t="str">
+      <c r="B14" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A14,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="94">
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B14)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="95"/>
+      <c r="H14" s="90"/>
       <c r="J14" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B14,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10189,19 +10191,19 @@
       <c r="A15" s="12">
         <v>9</v>
       </c>
-      <c r="B15" s="96" t="str">
+      <c r="B15" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A15,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="94">
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B15)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="95"/>
+      <c r="H15" s="90"/>
       <c r="J15" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B15,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10235,19 +10237,19 @@
       <c r="A16" s="12">
         <v>10</v>
       </c>
-      <c r="B16" s="96" t="str">
+      <c r="B16" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A16,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="94">
+      <c r="C16" s="80"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B16)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="95"/>
+      <c r="H16" s="90"/>
       <c r="J16" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B16,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10281,19 +10283,19 @@
       <c r="A17" s="12">
         <v>11</v>
       </c>
-      <c r="B17" s="96" t="str">
+      <c r="B17" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A17,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="94">
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B17)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="95"/>
+      <c r="H17" s="90"/>
       <c r="J17" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B17,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10327,19 +10329,19 @@
       <c r="A18" s="12">
         <v>12</v>
       </c>
-      <c r="B18" s="96" t="str">
+      <c r="B18" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A18,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="94">
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B18)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="95"/>
+      <c r="H18" s="90"/>
       <c r="J18" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B18,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10373,19 +10375,19 @@
       <c r="A19" s="12">
         <v>13</v>
       </c>
-      <c r="B19" s="96" t="str">
+      <c r="B19" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A19,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="94">
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B19)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="95"/>
+      <c r="H19" s="90"/>
       <c r="J19" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B19,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10419,19 +10421,19 @@
       <c r="A20" s="12">
         <v>14</v>
       </c>
-      <c r="B20" s="96" t="str">
+      <c r="B20" s="80" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A20,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="C20" s="96"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="94">
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="89">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B20)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="95"/>
+      <c r="H20" s="90"/>
       <c r="J20" s="15">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B20,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10465,19 +10467,19 @@
       <c r="A21" s="13">
         <v>15</v>
       </c>
-      <c r="B21" s="99" t="str">
+      <c r="B21" s="86" t="str">
         <f>IFERROR(VLOOKUP($A$4&amp;"-"&amp;$A21,ProjectTasks[[PRJTSKSEQ]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99"/>
-      <c r="E21" s="99"/>
-      <c r="F21" s="99"/>
-      <c r="G21" s="97">
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="95">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B21)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="98"/>
+      <c r="H21" s="96"/>
       <c r="J21" s="18">
         <f>SUMIFS(TaskTimings[Total Minutes],TaskTimings[PRJ],$A$4,TaskTimings[TSK],$B21,TaskTimings[Employee],J$5)</f>
         <v>0</v>
@@ -10509,91 +10511,67 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D23" s="86" t="s">
+      <c r="D23" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="87"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="86">
+      <c r="E23" s="99"/>
+      <c r="F23" s="100"/>
+      <c r="G23" s="98">
         <f>SUM(G7:H21)</f>
-        <v>1246.0000000000002</v>
-      </c>
-      <c r="H23" s="88"/>
-      <c r="J23" s="79">
+        <v>1966.0000000000002</v>
+      </c>
+      <c r="H23" s="100"/>
+      <c r="J23" s="93">
         <f>SUM(J7:J21)</f>
         <v>90</v>
       </c>
-      <c r="K23" s="79">
+      <c r="K23" s="93">
         <f t="shared" ref="K23:P23" si="0">SUM(K7:K21)</f>
         <v>0</v>
       </c>
-      <c r="L23" s="79">
+      <c r="L23" s="93">
         <f t="shared" si="0"/>
-        <v>1066.0000000000002</v>
-      </c>
-      <c r="M23" s="79">
+        <v>1786.0000000000002</v>
+      </c>
+      <c r="M23" s="93">
         <f t="shared" si="0"/>
         <v>89.999999999999915</v>
       </c>
-      <c r="N23" s="79">
+      <c r="N23" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O23" s="79">
+      <c r="O23" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P23" s="79">
+      <c r="P23" s="93">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="89"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="91"/>
-      <c r="G24" s="89"/>
-      <c r="H24" s="91"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="80"/>
-      <c r="M24" s="80"/>
-      <c r="N24" s="80"/>
-      <c r="O24" s="80"/>
-      <c r="P24" s="80"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="103"/>
+      <c r="G24" s="101"/>
+      <c r="H24" s="103"/>
+      <c r="J24" s="94"/>
+      <c r="K24" s="94"/>
+      <c r="L24" s="94"/>
+      <c r="M24" s="94"/>
+      <c r="N24" s="94"/>
+      <c r="O24" s="94"/>
+      <c r="P24" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A1:E3"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B5:F6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
     <mergeCell ref="J2:L3"/>
     <mergeCell ref="D23:F24"/>
     <mergeCell ref="G23:H24"/>
@@ -10610,12 +10588,36 @@
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="B20:F20"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B5:F6"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:E3">
@@ -10639,16 +10641,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="F1" s="108" t="s">
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="F1" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="108"/>
+      <c r="G1" s="125"/>
       <c r="I1" s="28" t="s">
         <v>41</v>
       </c>
@@ -10668,19 +10670,19 @@
       <c r="U1" s="21"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="106"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="F2" s="107">
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="F2" s="124">
         <v>43430</v>
       </c>
-      <c r="G2" s="107"/>
-      <c r="I2" s="124">
+      <c r="G2" s="124"/>
+      <c r="I2" s="104">
         <f>SUM(I7:I30)</f>
         <v>1696.0000000000002</v>
       </c>
-      <c r="J2" s="118" t="str">
+      <c r="J2" s="106" t="str">
         <f>TEXT($I$2/1440,"H:mm")</f>
         <v>4:16</v>
       </c>
@@ -10697,14 +10699,14 @@
       <c r="U2" s="21"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="106"/>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="I3" s="125"/>
-      <c r="J3" s="119"/>
+      <c r="A3" s="123"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="107"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
       <c r="M3" s="21"/>
@@ -10718,41 +10720,41 @@
       <c r="U3" s="21"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="K4" s="85" t="s">
+      <c r="K4" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>1</v>
       </c>
-      <c r="B6" s="105"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
       <c r="J6" s="25"/>
       <c r="K6" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="115" t="s">
+      <c r="L6" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="115"/>
+      <c r="M6" s="114"/>
       <c r="N6" s="35" t="s">
         <v>41</v>
       </c>
@@ -10767,23 +10769,23 @@
       <c r="A7" s="14">
         <v>2</v>
       </c>
-      <c r="B7" s="109">
+      <c r="B7" s="126">
         <f>$F$2</f>
         <v>43430</v>
       </c>
-      <c r="C7" s="81"/>
-      <c r="D7" s="110" t="str">
+      <c r="C7" s="87"/>
+      <c r="D7" s="127" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$7&amp;"/"&amp;$A6,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Discussion for ticketing modification</v>
       </c>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
       <c r="H7" s="23">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$7&amp;"/"&amp;$A6,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>90</v>
       </c>
-      <c r="I7" s="117">
+      <c r="I7" s="116">
         <f>SUM(H7:H10)</f>
         <v>330.99999999999994</v>
       </c>
@@ -10791,11 +10793,11 @@
       <c r="K7" s="72">
         <v>1</v>
       </c>
-      <c r="L7" s="120" t="str">
+      <c r="L7" s="108" t="str">
         <f>IFERROR(VLOOKUP($K7,$X$7:$Y$30,2,0),"")</f>
         <v>TKT</v>
       </c>
-      <c r="M7" s="120"/>
+      <c r="M7" s="108"/>
       <c r="N7" s="74">
         <f>SUMIFS($AB$7:$AB$30,$Y$7:$Y$30,$L7)</f>
         <v>1636.0000000000002</v>
@@ -10843,29 +10845,29 @@
       <c r="A8" s="14">
         <v>3</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="111" t="str">
+      <c r="B8" s="85"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$7&amp;"/"&amp;$A7,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Database Analysis from Old Project</v>
       </c>
-      <c r="E8" s="111"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="111"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="117"/>
+      <c r="G8" s="117"/>
       <c r="H8" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$7&amp;"/"&amp;$A7,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>121.00000000000006</v>
       </c>
-      <c r="I8" s="118"/>
+      <c r="I8" s="106"/>
       <c r="J8" s="25"/>
       <c r="K8" s="72">
         <v>2</v>
       </c>
-      <c r="L8" s="120" t="str">
+      <c r="L8" s="108" t="str">
         <f>IFERROR(VLOOKUP($K8,$X$7:$Y$30,2,0),"")</f>
         <v/>
       </c>
-      <c r="M8" s="120"/>
+      <c r="M8" s="108"/>
       <c r="N8" s="74">
         <f>SUMIFS($AB$7:$AB$30,$Y$7:$Y$30,$L8)</f>
         <v>0</v>
@@ -10913,29 +10915,29 @@
       <c r="A9" s="14">
         <v>4</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="111" t="str">
+      <c r="B9" s="85"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$7&amp;"/"&amp;$A8,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Database Analysis from Old Project</v>
       </c>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="111"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="117"/>
+      <c r="G9" s="117"/>
       <c r="H9" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$7&amp;"/"&amp;$A8,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>119.99999999999989</v>
       </c>
-      <c r="I9" s="118"/>
+      <c r="I9" s="106"/>
       <c r="J9" s="25"/>
       <c r="K9" s="72">
         <v>3</v>
       </c>
-      <c r="L9" s="120" t="str">
+      <c r="L9" s="108" t="str">
         <f>IFERROR(VLOOKUP($K9,$X$7:$Y$30,2,0),"")</f>
         <v/>
       </c>
-      <c r="M9" s="120"/>
+      <c r="M9" s="108"/>
       <c r="N9" s="74">
         <f>SUMIFS($AB$7:$AB$30,$Y$7:$Y$30,$L9)</f>
         <v>0</v>
@@ -10983,29 +10985,29 @@
       <c r="A10" s="14">
         <v>1</v>
       </c>
-      <c r="B10" s="93"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="111" t="str">
+      <c r="B10" s="85"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$7&amp;"/"&amp;$A9,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="111"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="117"/>
+      <c r="G10" s="117"/>
       <c r="H10" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$7&amp;"/"&amp;$A9,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="118"/>
+      <c r="I10" s="106"/>
       <c r="J10" s="25"/>
       <c r="K10" s="72">
         <v>4</v>
       </c>
-      <c r="L10" s="120" t="str">
+      <c r="L10" s="108" t="str">
         <f>IFERROR(VLOOKUP($K10,$X$7:$Y$30,2,0),"")</f>
         <v/>
       </c>
-      <c r="M10" s="120"/>
+      <c r="M10" s="108"/>
       <c r="N10" s="74">
         <f>SUMIFS($AB$7:$AB$30,$Y$7:$Y$30,$L10)</f>
         <v>0</v>
@@ -11053,23 +11055,23 @@
       <c r="A11" s="14">
         <v>2</v>
       </c>
-      <c r="B11" s="112">
+      <c r="B11" s="118">
         <f>B7+1</f>
         <v>43431</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="111" t="str">
+      <c r="C11" s="88"/>
+      <c r="D11" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$11&amp;"/"&amp;$A10,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Database Analysis from Old Project</v>
       </c>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="111"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
       <c r="H11" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$11&amp;"/"&amp;$A10,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>135</v>
       </c>
-      <c r="I11" s="118">
+      <c r="I11" s="106">
         <f t="shared" ref="I11" si="2">SUM(H11:H14)</f>
         <v>135</v>
       </c>
@@ -11077,11 +11079,11 @@
       <c r="K11" s="73">
         <v>5</v>
       </c>
-      <c r="L11" s="123" t="str">
+      <c r="L11" s="111" t="str">
         <f>IFERROR(VLOOKUP($K11,$X$7:$Y$30,2,0),"")</f>
         <v/>
       </c>
-      <c r="M11" s="123"/>
+      <c r="M11" s="111"/>
       <c r="N11" s="75">
         <f>SUMIFS($AB$7:$AB$30,$Y$7:$Y$30,$L11)</f>
         <v>0</v>
@@ -11129,20 +11131,20 @@
       <c r="A12" s="14">
         <v>3</v>
       </c>
-      <c r="B12" s="93"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="111" t="str">
+      <c r="B12" s="85"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$11&amp;"/"&amp;$A11,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="117"/>
+      <c r="G12" s="117"/>
       <c r="H12" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$11&amp;"/"&amp;$A11,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="118"/>
+      <c r="I12" s="106"/>
       <c r="J12" s="25"/>
       <c r="K12" s="25"/>
       <c r="L12" s="25"/>
@@ -11191,27 +11193,27 @@
       <c r="A13" s="14">
         <v>4</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="111" t="str">
+      <c r="B13" s="85"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$11&amp;"/"&amp;$A12,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
       <c r="H13" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$11&amp;"/"&amp;$A12,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="118"/>
+      <c r="I13" s="106"/>
       <c r="J13" s="25"/>
-      <c r="K13" s="104" t="s">
+      <c r="K13" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="L13" s="104"/>
-      <c r="M13" s="104"/>
-      <c r="N13" s="104"/>
+      <c r="L13" s="121"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
       <c r="Q13" s="25"/>
@@ -11255,25 +11257,25 @@
       <c r="A14" s="14">
         <v>1</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="111" t="str">
+      <c r="B14" s="85"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$11&amp;"/"&amp;$A13,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="111"/>
+      <c r="E14" s="117"/>
+      <c r="F14" s="117"/>
+      <c r="G14" s="117"/>
       <c r="H14" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$11&amp;"/"&amp;$A13,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="118"/>
+      <c r="I14" s="106"/>
       <c r="J14" s="25"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="105"/>
-      <c r="N14" s="105"/>
+      <c r="K14" s="122"/>
+      <c r="L14" s="122"/>
+      <c r="M14" s="122"/>
+      <c r="N14" s="122"/>
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
@@ -11317,37 +11319,37 @@
       <c r="A15" s="14">
         <v>2</v>
       </c>
-      <c r="B15" s="112">
+      <c r="B15" s="118">
         <f>B11+1</f>
         <v>43432</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="111" t="str">
+      <c r="C15" s="88"/>
+      <c r="D15" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$15&amp;"/"&amp;$A14,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Note down table relations</v>
       </c>
-      <c r="E15" s="111"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="111"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="117"/>
+      <c r="G15" s="117"/>
       <c r="H15" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$15&amp;"/"&amp;$A14,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>380.00000000000011</v>
       </c>
-      <c r="I15" s="118">
+      <c r="I15" s="106">
         <f t="shared" ref="I15" si="3">SUM(H15:H18)</f>
         <v>380.00000000000011</v>
       </c>
       <c r="J15" s="25"/>
-      <c r="K15" s="121" t="s">
+      <c r="K15" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="L15" s="122"/>
-      <c r="M15" s="122" t="s">
+      <c r="L15" s="112"/>
+      <c r="M15" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="N15" s="122"/>
-      <c r="O15" s="122"/>
-      <c r="P15" s="122"/>
+      <c r="N15" s="112"/>
+      <c r="O15" s="112"/>
+      <c r="P15" s="112"/>
       <c r="Q15" s="23" t="s">
         <v>42</v>
       </c>
@@ -11393,40 +11395,40 @@
       <c r="A16" s="14">
         <v>3</v>
       </c>
-      <c r="B16" s="93"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="111" t="str">
+      <c r="B16" s="85"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$15&amp;"/"&amp;$A15,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E16" s="111"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="117"/>
       <c r="H16" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$15&amp;"/"&amp;$A15,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="118"/>
+      <c r="I16" s="106"/>
       <c r="J16" s="26">
         <v>1</v>
       </c>
-      <c r="K16" s="126" t="str">
+      <c r="K16" s="109" t="str">
         <f>VLOOKUP(1,$K$7:$M$11,2,0)</f>
         <v>TKT</v>
       </c>
-      <c r="L16" s="94"/>
-      <c r="M16" s="120" t="str">
+      <c r="L16" s="89"/>
+      <c r="M16" s="108" t="str">
         <f>IF($K$16="","",IFERROR(VLOOKUP($K$16&amp;"/"&amp;$J16,$Z$7:$AA$30,2,0),""))</f>
         <v>Discussion for ticketing modification</v>
       </c>
-      <c r="N16" s="120"/>
-      <c r="O16" s="120"/>
-      <c r="P16" s="120"/>
+      <c r="N16" s="108"/>
+      <c r="O16" s="108"/>
+      <c r="P16" s="108"/>
       <c r="Q16" s="22">
         <f>IF($M16="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$16&amp;"/"&amp;$M16))</f>
         <v>90</v>
       </c>
-      <c r="R16" s="118">
+      <c r="R16" s="106">
         <f>SUM(Q16:Q19)</f>
         <v>1636.0000000000002</v>
       </c>
@@ -11469,37 +11471,37 @@
       <c r="A17" s="14">
         <v>4</v>
       </c>
-      <c r="B17" s="93"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="111" t="str">
+      <c r="B17" s="85"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$15&amp;"/"&amp;$A16,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E17" s="111"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="117"/>
       <c r="H17" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$15&amp;"/"&amp;$A16,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="118"/>
+      <c r="I17" s="106"/>
       <c r="J17" s="26">
         <v>2</v>
       </c>
-      <c r="K17" s="126"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="120" t="str">
+      <c r="K17" s="109"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="108" t="str">
         <f>IF($K$16="","",IFERROR(VLOOKUP($K$16&amp;"/"&amp;$J17,$Z$7:$AA$30,2,0),""))</f>
         <v>Database Analysis from Old Project</v>
       </c>
-      <c r="N17" s="120"/>
-      <c r="O17" s="120"/>
-      <c r="P17" s="120"/>
+      <c r="N17" s="108"/>
+      <c r="O17" s="108"/>
+      <c r="P17" s="108"/>
       <c r="Q17" s="22">
         <f>IF($M17="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$16&amp;"/"&amp;$M17))</f>
         <v>375.99999999999994</v>
       </c>
-      <c r="R17" s="118"/>
+      <c r="R17" s="106"/>
       <c r="S17" s="31"/>
       <c r="T17" s="32"/>
       <c r="U17" s="14">
@@ -11539,37 +11541,37 @@
       <c r="A18" s="14">
         <v>1</v>
       </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="111" t="str">
+      <c r="B18" s="85"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$15&amp;"/"&amp;$A17,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="117"/>
       <c r="H18" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$15&amp;"/"&amp;$A17,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="118"/>
+      <c r="I18" s="106"/>
       <c r="J18" s="26">
         <v>3</v>
       </c>
-      <c r="K18" s="126"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="120" t="str">
+      <c r="K18" s="109"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="108" t="str">
         <f>IF($K$16="","",IFERROR(VLOOKUP($K$16&amp;"/"&amp;$J18,$Z$7:$AA$30,2,0),""))</f>
         <v>Note down table relations</v>
       </c>
-      <c r="N18" s="120"/>
-      <c r="O18" s="120"/>
-      <c r="P18" s="120"/>
+      <c r="N18" s="108"/>
+      <c r="O18" s="108"/>
+      <c r="P18" s="108"/>
       <c r="Q18" s="22">
         <f>IF($M18="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$16&amp;"/"&amp;$M18))</f>
         <v>510.00000000000011</v>
       </c>
-      <c r="R18" s="118"/>
+      <c r="R18" s="106"/>
       <c r="S18" s="31"/>
       <c r="T18" s="32"/>
       <c r="U18" s="14">
@@ -11609,43 +11611,43 @@
       <c r="A19" s="14">
         <v>2</v>
       </c>
-      <c r="B19" s="112">
+      <c r="B19" s="118">
         <f>B15+1</f>
         <v>43433</v>
       </c>
-      <c r="C19" s="82"/>
-      <c r="D19" s="111" t="str">
+      <c r="C19" s="88"/>
+      <c r="D19" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$19&amp;"/"&amp;$A18,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Note down table relations</v>
       </c>
-      <c r="E19" s="111"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="111"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+      <c r="G19" s="117"/>
       <c r="H19" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$19&amp;"/"&amp;$A18,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>130.00000000000003</v>
       </c>
-      <c r="I19" s="118">
+      <c r="I19" s="106">
         <f t="shared" ref="I19" si="4">SUM(H19:H22)</f>
         <v>250.00000000000009</v>
       </c>
       <c r="J19" s="26">
         <v>4</v>
       </c>
-      <c r="K19" s="126"/>
-      <c r="L19" s="94"/>
-      <c r="M19" s="120" t="str">
+      <c r="K19" s="109"/>
+      <c r="L19" s="89"/>
+      <c r="M19" s="108" t="str">
         <f>IF($K$16="","",IFERROR(VLOOKUP($K$16&amp;"/"&amp;$J19,$Z$7:$AA$30,2,0),""))</f>
         <v>Entering table details into excel sheet</v>
       </c>
-      <c r="N19" s="120"/>
-      <c r="O19" s="120"/>
-      <c r="P19" s="120"/>
+      <c r="N19" s="108"/>
+      <c r="O19" s="108"/>
+      <c r="P19" s="108"/>
       <c r="Q19" s="22">
         <f>IF($M19="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$16&amp;"/"&amp;$M19))</f>
         <v>660.00000000000023</v>
       </c>
-      <c r="R19" s="118"/>
+      <c r="R19" s="106"/>
       <c r="S19" s="31"/>
       <c r="T19" s="32"/>
       <c r="U19" s="14">
@@ -11685,40 +11687,40 @@
       <c r="A20" s="14">
         <v>3</v>
       </c>
-      <c r="B20" s="93"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="111" t="str">
+      <c r="B20" s="85"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$19&amp;"/"&amp;$A19,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Entering table details into excel sheet</v>
       </c>
-      <c r="E20" s="111"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
+      <c r="G20" s="117"/>
       <c r="H20" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$19&amp;"/"&amp;$A19,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>120.00000000000006</v>
       </c>
-      <c r="I20" s="118"/>
+      <c r="I20" s="106"/>
       <c r="J20" s="26">
         <v>1</v>
       </c>
-      <c r="K20" s="126" t="str">
+      <c r="K20" s="109" t="str">
         <f>VLOOKUP(2,$K$7:$M$11,2,0)</f>
         <v/>
       </c>
-      <c r="L20" s="94"/>
-      <c r="M20" s="120" t="str">
+      <c r="L20" s="89"/>
+      <c r="M20" s="108" t="str">
         <f>IF($K$20="","",IFERROR(VLOOKUP($K$20&amp;"/"&amp;$J20,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N20" s="120"/>
-      <c r="O20" s="120"/>
-      <c r="P20" s="120"/>
+      <c r="N20" s="108"/>
+      <c r="O20" s="108"/>
+      <c r="P20" s="108"/>
       <c r="Q20" s="22" t="str">
         <f>IF($M20="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$20&amp;"/"&amp;$M20))</f>
         <v/>
       </c>
-      <c r="R20" s="118">
+      <c r="R20" s="106">
         <f t="shared" ref="R20" si="5">SUM(Q20:Q23)</f>
         <v>0</v>
       </c>
@@ -11761,37 +11763,37 @@
       <c r="A21" s="14">
         <v>4</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="111" t="str">
+      <c r="B21" s="85"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$19&amp;"/"&amp;$A20,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E21" s="111"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="111"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
       <c r="H21" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$19&amp;"/"&amp;$A20,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I21" s="118"/>
+      <c r="I21" s="106"/>
       <c r="J21" s="26">
         <v>2</v>
       </c>
-      <c r="K21" s="126"/>
-      <c r="L21" s="94"/>
-      <c r="M21" s="120" t="str">
+      <c r="K21" s="109"/>
+      <c r="L21" s="89"/>
+      <c r="M21" s="108" t="str">
         <f>IF($K$20="","",IFERROR(VLOOKUP($K$20&amp;"/"&amp;$J21,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N21" s="120"/>
-      <c r="O21" s="120"/>
-      <c r="P21" s="120"/>
+      <c r="N21" s="108"/>
+      <c r="O21" s="108"/>
+      <c r="P21" s="108"/>
       <c r="Q21" s="22" t="str">
         <f>IF($M21="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$20&amp;"/"&amp;$M21))</f>
         <v/>
       </c>
-      <c r="R21" s="118"/>
+      <c r="R21" s="106"/>
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
       <c r="U21" s="14">
@@ -11831,37 +11833,37 @@
       <c r="A22" s="14">
         <v>1</v>
       </c>
-      <c r="B22" s="93"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="111" t="str">
+      <c r="B22" s="85"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$19&amp;"/"&amp;$A21,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="111"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="117"/>
       <c r="H22" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$19&amp;"/"&amp;$A21,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="118"/>
+      <c r="I22" s="106"/>
       <c r="J22" s="26">
         <v>3</v>
       </c>
-      <c r="K22" s="126"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="120" t="str">
+      <c r="K22" s="109"/>
+      <c r="L22" s="89"/>
+      <c r="M22" s="108" t="str">
         <f>IF($K$20="","",IFERROR(VLOOKUP($K$20&amp;"/"&amp;$J22,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N22" s="120"/>
-      <c r="O22" s="120"/>
-      <c r="P22" s="120"/>
+      <c r="N22" s="108"/>
+      <c r="O22" s="108"/>
+      <c r="P22" s="108"/>
       <c r="Q22" s="22" t="str">
         <f>IF($M22="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$20&amp;"/"&amp;$M22))</f>
         <v/>
       </c>
-      <c r="R22" s="118"/>
+      <c r="R22" s="106"/>
       <c r="S22" s="25"/>
       <c r="T22" s="25"/>
       <c r="U22" s="14">
@@ -11901,43 +11903,43 @@
       <c r="A23" s="14">
         <v>2</v>
       </c>
-      <c r="B23" s="112">
+      <c r="B23" s="118">
         <f>B19+1</f>
         <v>43434</v>
       </c>
-      <c r="C23" s="82"/>
-      <c r="D23" s="111" t="str">
+      <c r="C23" s="88"/>
+      <c r="D23" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$23&amp;"/"&amp;$A22,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Entering table details into excel sheet</v>
       </c>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="111"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
       <c r="H23" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$23&amp;"/"&amp;$A22,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>204.99999999999991</v>
       </c>
-      <c r="I23" s="118">
+      <c r="I23" s="106">
         <f t="shared" ref="I23" si="6">SUM(H23:H26)</f>
         <v>389.99999999999989</v>
       </c>
       <c r="J23" s="26">
         <v>4</v>
       </c>
-      <c r="K23" s="126"/>
-      <c r="L23" s="94"/>
-      <c r="M23" s="120" t="str">
+      <c r="K23" s="109"/>
+      <c r="L23" s="89"/>
+      <c r="M23" s="108" t="str">
         <f>IF($K$20="","",IFERROR(VLOOKUP($K$20&amp;"/"&amp;$J23,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N23" s="120"/>
-      <c r="O23" s="120"/>
-      <c r="P23" s="120"/>
+      <c r="N23" s="108"/>
+      <c r="O23" s="108"/>
+      <c r="P23" s="108"/>
       <c r="Q23" s="22" t="str">
         <f>IF($M23="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$20&amp;"/"&amp;$M23))</f>
         <v/>
       </c>
-      <c r="R23" s="118"/>
+      <c r="R23" s="106"/>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
       <c r="U23" s="14">
@@ -11977,40 +11979,40 @@
       <c r="A24" s="14">
         <v>3</v>
       </c>
-      <c r="B24" s="93"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="111" t="str">
+      <c r="B24" s="85"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$23&amp;"/"&amp;$A23,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Entering table details into excel sheet</v>
       </c>
-      <c r="E24" s="111"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="111"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="117"/>
       <c r="H24" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$23&amp;"/"&amp;$A23,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>125.00000000000003</v>
       </c>
-      <c r="I24" s="118"/>
+      <c r="I24" s="106"/>
       <c r="J24" s="26">
         <v>1</v>
       </c>
-      <c r="K24" s="126" t="str">
+      <c r="K24" s="109" t="str">
         <f>VLOOKUP(3,$K$7:$M$11,2,0)</f>
         <v/>
       </c>
-      <c r="L24" s="94"/>
-      <c r="M24" s="120" t="str">
+      <c r="L24" s="89"/>
+      <c r="M24" s="108" t="str">
         <f>IF($K$24="","",IFERROR(VLOOKUP($K$24&amp;"/"&amp;$J24,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N24" s="120"/>
-      <c r="O24" s="120"/>
-      <c r="P24" s="120"/>
+      <c r="N24" s="108"/>
+      <c r="O24" s="108"/>
+      <c r="P24" s="108"/>
       <c r="Q24" s="22" t="str">
         <f>IF($M24="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$24&amp;"/"&amp;$M24))</f>
         <v/>
       </c>
-      <c r="R24" s="118">
+      <c r="R24" s="106">
         <f t="shared" ref="R24" si="7">SUM(Q24:Q27)</f>
         <v>0</v>
       </c>
@@ -12053,37 +12055,37 @@
       <c r="A25" s="14">
         <v>4</v>
       </c>
-      <c r="B25" s="93"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="111" t="str">
+      <c r="B25" s="85"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$23&amp;"/"&amp;$A24,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TEEBPD/Inhouse Testing</v>
       </c>
-      <c r="E25" s="111"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="111"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="117"/>
+      <c r="G25" s="117"/>
       <c r="H25" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$23&amp;"/"&amp;$A24,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>59.999999999999943</v>
       </c>
-      <c r="I25" s="118"/>
+      <c r="I25" s="106"/>
       <c r="J25" s="26">
         <v>2</v>
       </c>
-      <c r="K25" s="126"/>
-      <c r="L25" s="94"/>
-      <c r="M25" s="120" t="str">
+      <c r="K25" s="109"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="108" t="str">
         <f>IF($K$24="","",IFERROR(VLOOKUP($K$24&amp;"/"&amp;$J25,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N25" s="120"/>
-      <c r="O25" s="120"/>
-      <c r="P25" s="120"/>
+      <c r="N25" s="108"/>
+      <c r="O25" s="108"/>
+      <c r="P25" s="108"/>
       <c r="Q25" s="22" t="str">
         <f>IF($M25="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$24&amp;"/"&amp;$M25))</f>
         <v/>
       </c>
-      <c r="R25" s="118"/>
+      <c r="R25" s="106"/>
       <c r="S25" s="25"/>
       <c r="T25" s="25"/>
       <c r="U25" s="14">
@@ -12123,37 +12125,37 @@
       <c r="A26" s="14">
         <v>1</v>
       </c>
-      <c r="B26" s="93"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="111" t="str">
+      <c r="B26" s="85"/>
+      <c r="C26" s="88"/>
+      <c r="D26" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$23&amp;"/"&amp;$A25,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E26" s="111"/>
-      <c r="F26" s="111"/>
-      <c r="G26" s="111"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="117"/>
       <c r="H26" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$23&amp;"/"&amp;$A25,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="118"/>
+      <c r="I26" s="106"/>
       <c r="J26" s="26">
         <v>3</v>
       </c>
-      <c r="K26" s="126"/>
-      <c r="L26" s="94"/>
-      <c r="M26" s="120" t="str">
+      <c r="K26" s="109"/>
+      <c r="L26" s="89"/>
+      <c r="M26" s="108" t="str">
         <f>IF($K$24="","",IFERROR(VLOOKUP($K$24&amp;"/"&amp;$J26,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N26" s="120"/>
-      <c r="O26" s="120"/>
-      <c r="P26" s="120"/>
+      <c r="N26" s="108"/>
+      <c r="O26" s="108"/>
+      <c r="P26" s="108"/>
       <c r="Q26" s="22" t="str">
         <f>IF($M26="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$24&amp;"/"&amp;$M26))</f>
         <v/>
       </c>
-      <c r="R26" s="118"/>
+      <c r="R26" s="106"/>
       <c r="S26" s="25"/>
       <c r="T26" s="25"/>
       <c r="U26" s="14">
@@ -12193,43 +12195,43 @@
       <c r="A27" s="14">
         <v>2</v>
       </c>
-      <c r="B27" s="112">
+      <c r="B27" s="118">
         <f>B23+1</f>
         <v>43435</v>
       </c>
-      <c r="C27" s="82"/>
-      <c r="D27" s="111" t="str">
+      <c r="C27" s="88"/>
+      <c r="D27" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$27&amp;"/"&amp;$A26,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Entering table details into excel sheet</v>
       </c>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
       <c r="H27" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$27&amp;"/"&amp;$A26,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>90.000000000000085</v>
       </c>
-      <c r="I27" s="118">
+      <c r="I27" s="106">
         <f t="shared" ref="I27" si="8">SUM(H27:H30)</f>
         <v>210.00000000000014</v>
       </c>
       <c r="J27" s="26">
         <v>4</v>
       </c>
-      <c r="K27" s="126"/>
-      <c r="L27" s="94"/>
-      <c r="M27" s="120" t="str">
+      <c r="K27" s="109"/>
+      <c r="L27" s="89"/>
+      <c r="M27" s="108" t="str">
         <f>IF($K$24="","",IFERROR(VLOOKUP($K$24&amp;"/"&amp;$J27,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N27" s="120"/>
-      <c r="O27" s="120"/>
-      <c r="P27" s="120"/>
+      <c r="N27" s="108"/>
+      <c r="O27" s="108"/>
+      <c r="P27" s="108"/>
       <c r="Q27" s="22" t="str">
         <f>IF($M27="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$24&amp;"/"&amp;$M27))</f>
         <v/>
       </c>
-      <c r="R27" s="118"/>
+      <c r="R27" s="106"/>
       <c r="S27" s="25"/>
       <c r="T27" s="25"/>
       <c r="U27" s="14">
@@ -12269,40 +12271,40 @@
       <c r="A28" s="14">
         <v>3</v>
       </c>
-      <c r="B28" s="93"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="111" t="str">
+      <c r="B28" s="85"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$27&amp;"/"&amp;$A27,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v>TKT/Entering table details into excel sheet</v>
       </c>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="111"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
       <c r="H28" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$27&amp;"/"&amp;$A27,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>120.00000000000006</v>
       </c>
-      <c r="I28" s="118"/>
+      <c r="I28" s="106"/>
       <c r="J28" s="26">
         <v>1</v>
       </c>
-      <c r="K28" s="126" t="str">
+      <c r="K28" s="109" t="str">
         <f>VLOOKUP(4,$K$7:$M$11,2,0)</f>
         <v/>
       </c>
-      <c r="L28" s="94"/>
-      <c r="M28" s="120" t="str">
+      <c r="L28" s="89"/>
+      <c r="M28" s="108" t="str">
         <f>IF($K$28="","",IFERROR(VLOOKUP($K$28&amp;"/"&amp;$J28,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N28" s="120"/>
-      <c r="O28" s="120"/>
-      <c r="P28" s="120"/>
+      <c r="N28" s="108"/>
+      <c r="O28" s="108"/>
+      <c r="P28" s="108"/>
       <c r="Q28" s="22" t="str">
         <f>IF($M28="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$28&amp;"/"&amp;$M28))</f>
         <v/>
       </c>
-      <c r="R28" s="118">
+      <c r="R28" s="106">
         <f t="shared" ref="R28" si="9">SUM(Q28:Q31)</f>
         <v>0</v>
       </c>
@@ -12345,37 +12347,37 @@
       <c r="A29" s="14">
         <v>4</v>
       </c>
-      <c r="B29" s="93"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="111" t="str">
+      <c r="B29" s="85"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="117" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$27&amp;"/"&amp;$A28,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E29" s="111"/>
-      <c r="F29" s="111"/>
-      <c r="G29" s="111"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="117"/>
       <c r="H29" s="22">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$27&amp;"/"&amp;$A28,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="118"/>
+      <c r="I29" s="106"/>
       <c r="J29" s="26">
         <v>2</v>
       </c>
-      <c r="K29" s="126"/>
-      <c r="L29" s="94"/>
-      <c r="M29" s="120" t="str">
+      <c r="K29" s="109"/>
+      <c r="L29" s="89"/>
+      <c r="M29" s="108" t="str">
         <f>IF($K$28="","",IFERROR(VLOOKUP($K$28&amp;"/"&amp;$J29,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N29" s="120"/>
-      <c r="O29" s="120"/>
-      <c r="P29" s="120"/>
+      <c r="N29" s="108"/>
+      <c r="O29" s="108"/>
+      <c r="P29" s="108"/>
       <c r="Q29" s="22" t="str">
         <f>IF($M29="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$28&amp;"/"&amp;$M29))</f>
         <v/>
       </c>
-      <c r="R29" s="118"/>
+      <c r="R29" s="106"/>
       <c r="S29" s="25"/>
       <c r="T29" s="25"/>
       <c r="U29" s="14">
@@ -12412,37 +12414,37 @@
       </c>
     </row>
     <row r="30" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="113"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="116" t="str">
+      <c r="B30" s="119"/>
+      <c r="C30" s="120"/>
+      <c r="D30" s="115" t="str">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$27&amp;"/"&amp;$A29,TaskTimings[[EmployeeDateSeqCode]:[Task]],2,0),"")</f>
         <v/>
       </c>
-      <c r="E30" s="116"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
+      <c r="E30" s="115"/>
+      <c r="F30" s="115"/>
+      <c r="G30" s="115"/>
       <c r="H30" s="24">
         <f>IFERROR(VLOOKUP($A$1&amp;"/"&amp;$B$27&amp;"/"&amp;$A29,TaskTimings[[EmployeeDateSeqCode]:[Total Minutes]],7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="119"/>
+      <c r="I30" s="107"/>
       <c r="J30" s="26">
         <v>3</v>
       </c>
-      <c r="K30" s="126"/>
-      <c r="L30" s="94"/>
-      <c r="M30" s="120" t="str">
+      <c r="K30" s="109"/>
+      <c r="L30" s="89"/>
+      <c r="M30" s="108" t="str">
         <f>IF($K$28="","",IFERROR(VLOOKUP($K$28&amp;"/"&amp;$J30,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N30" s="120"/>
-      <c r="O30" s="120"/>
-      <c r="P30" s="120"/>
+      <c r="N30" s="108"/>
+      <c r="O30" s="108"/>
+      <c r="P30" s="108"/>
       <c r="Q30" s="22" t="str">
         <f>IF($M30="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$28&amp;"/"&amp;$M30))</f>
         <v/>
       </c>
-      <c r="R30" s="118"/>
+      <c r="R30" s="106"/>
       <c r="U30" s="14">
         <f>IF(COUNTIFS($D$6:$D30,D30)=1,1,0)</f>
         <v>0</v>
@@ -12480,42 +12482,42 @@
       <c r="J31" s="26">
         <v>4</v>
       </c>
-      <c r="K31" s="126"/>
-      <c r="L31" s="94"/>
-      <c r="M31" s="120" t="str">
+      <c r="K31" s="109"/>
+      <c r="L31" s="89"/>
+      <c r="M31" s="108" t="str">
         <f>IF($K$28="","",IFERROR(VLOOKUP($K$28&amp;"/"&amp;$J31,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N31" s="120"/>
-      <c r="O31" s="120"/>
-      <c r="P31" s="120"/>
+      <c r="N31" s="108"/>
+      <c r="O31" s="108"/>
+      <c r="P31" s="108"/>
       <c r="Q31" s="22" t="str">
         <f>IF($M31="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$28&amp;"/"&amp;$M31))</f>
         <v/>
       </c>
-      <c r="R31" s="118"/>
+      <c r="R31" s="106"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J32" s="26">
         <v>1</v>
       </c>
-      <c r="K32" s="126" t="str">
+      <c r="K32" s="109" t="str">
         <f>VLOOKUP(5,$K$7:$M$11,2,0)</f>
         <v/>
       </c>
-      <c r="L32" s="94"/>
-      <c r="M32" s="120" t="str">
+      <c r="L32" s="89"/>
+      <c r="M32" s="108" t="str">
         <f>IF($K$32="","",IFERROR(VLOOKUP($K$32&amp;"/"&amp;$J32,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N32" s="120"/>
-      <c r="O32" s="120"/>
-      <c r="P32" s="120"/>
+      <c r="N32" s="108"/>
+      <c r="O32" s="108"/>
+      <c r="P32" s="108"/>
       <c r="Q32" s="22" t="str">
         <f>IF($M32="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$32&amp;"/"&amp;$M32))</f>
         <v/>
       </c>
-      <c r="R32" s="118">
+      <c r="R32" s="106">
         <f t="shared" ref="R32" si="10">SUM(Q32:Q35)</f>
         <v>0</v>
       </c>
@@ -12524,61 +12526,127 @@
       <c r="J33" s="26">
         <v>2</v>
       </c>
-      <c r="K33" s="126"/>
-      <c r="L33" s="94"/>
-      <c r="M33" s="120" t="str">
+      <c r="K33" s="109"/>
+      <c r="L33" s="89"/>
+      <c r="M33" s="108" t="str">
         <f>IF($K$32="","",IFERROR(VLOOKUP($K$32&amp;"/"&amp;$J33,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N33" s="120"/>
-      <c r="O33" s="120"/>
-      <c r="P33" s="120"/>
+      <c r="N33" s="108"/>
+      <c r="O33" s="108"/>
+      <c r="P33" s="108"/>
       <c r="Q33" s="22" t="str">
         <f>IF($M33="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$32&amp;"/"&amp;$M33))</f>
         <v/>
       </c>
-      <c r="R33" s="118"/>
+      <c r="R33" s="106"/>
     </row>
     <row r="34" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J34" s="26">
         <v>3</v>
       </c>
-      <c r="K34" s="126"/>
-      <c r="L34" s="94"/>
-      <c r="M34" s="120" t="str">
+      <c r="K34" s="109"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="108" t="str">
         <f>IF($K$32="","",IFERROR(VLOOKUP($K$32&amp;"/"&amp;$J34,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N34" s="120"/>
-      <c r="O34" s="120"/>
-      <c r="P34" s="120"/>
+      <c r="N34" s="108"/>
+      <c r="O34" s="108"/>
+      <c r="P34" s="108"/>
       <c r="Q34" s="22" t="str">
         <f>IF($M34="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$32&amp;"/"&amp;$M34))</f>
         <v/>
       </c>
-      <c r="R34" s="118"/>
+      <c r="R34" s="106"/>
     </row>
     <row r="35" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J35" s="26">
         <v>4</v>
       </c>
-      <c r="K35" s="127"/>
-      <c r="L35" s="97"/>
-      <c r="M35" s="123" t="str">
+      <c r="K35" s="110"/>
+      <c r="L35" s="95"/>
+      <c r="M35" s="111" t="str">
         <f>IF($K$32="","",IFERROR(VLOOKUP($K$32&amp;"/"&amp;$J35,$Z$7:$AA$30,2,0),""))</f>
         <v/>
       </c>
-      <c r="N35" s="123"/>
-      <c r="O35" s="123"/>
-      <c r="P35" s="123"/>
+      <c r="N35" s="111"/>
+      <c r="O35" s="111"/>
+      <c r="P35" s="111"/>
       <c r="Q35" s="24" t="str">
         <f>IF($M35="","",SUMIFS($H$7:$H$30,$D$7:$D$30,$K$32&amp;"/"&amp;$M35))</f>
         <v/>
       </c>
-      <c r="R35" s="119"/>
+      <c r="R35" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="K4:M5"/>
+    <mergeCell ref="K13:N14"/>
+    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B7:C10"/>
+    <mergeCell ref="B5:F6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="B11:C14"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="B15:C18"/>
+    <mergeCell ref="B19:C22"/>
+    <mergeCell ref="B23:C26"/>
+    <mergeCell ref="B27:C30"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="I19:I22"/>
+    <mergeCell ref="I23:I26"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="R16:R19"/>
+    <mergeCell ref="R20:R23"/>
+    <mergeCell ref="R24:R27"/>
+    <mergeCell ref="R28:R31"/>
+    <mergeCell ref="R32:R35"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="M30:P30"/>
+    <mergeCell ref="M31:P31"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="M22:P22"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="M32:P32"/>
@@ -12595,72 +12663,6 @@
     <mergeCell ref="M16:P16"/>
     <mergeCell ref="M17:P17"/>
     <mergeCell ref="M18:P18"/>
-    <mergeCell ref="M35:P35"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="R16:R19"/>
-    <mergeCell ref="R20:R23"/>
-    <mergeCell ref="R24:R27"/>
-    <mergeCell ref="R28:R31"/>
-    <mergeCell ref="R32:R35"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="M30:P30"/>
-    <mergeCell ref="M31:P31"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="I19:I22"/>
-    <mergeCell ref="I23:I26"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="B15:C18"/>
-    <mergeCell ref="B19:C22"/>
-    <mergeCell ref="B23:C26"/>
-    <mergeCell ref="B27:C30"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="K4:M5"/>
-    <mergeCell ref="K13:N14"/>
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B7:C10"/>
-    <mergeCell ref="B5:F6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="B11:C14"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:D3">

</xml_diff>